<commit_message>
Creacion de DataSet terminada, se puede empezar a hacer el modelo de ML
</commit_message>
<xml_diff>
--- a/DatosTrain.xlsx
+++ b/DatosTrain.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="2">
   <si>
     <t>1</t>
   </si>
@@ -351,13 +351,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q14"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -409,8 +409,14 @@
       <c r="Q1">
         <v>11621314.875</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1">
+        <v>5027</v>
+      </c>
+      <c r="S1">
+        <v>0.02472362494798537</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -462,8 +468,14 @@
       <c r="Q2">
         <v>12628841.25</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="R2">
+        <v>4989</v>
+      </c>
+      <c r="S2">
+        <v>0.03436524775970404</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -515,8 +527,14 @@
       <c r="Q3">
         <v>11346330.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3">
+        <v>5206</v>
+      </c>
+      <c r="S3">
+        <v>0.02890479927642864</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -568,8 +586,14 @@
       <c r="Q4">
         <v>11158715.375</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="R4">
+        <v>4247</v>
+      </c>
+      <c r="S4">
+        <v>0.03042682410642743</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -621,8 +645,14 @@
       <c r="Q5">
         <v>11691305.41666667</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="R5">
+        <v>5650</v>
+      </c>
+      <c r="S5">
+        <v>0.03003712341895088</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -674,8 +704,14 @@
       <c r="Q6">
         <v>11454550.08333333</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="R6">
+        <v>5479</v>
+      </c>
+      <c r="S6">
+        <v>0.02699268327350968</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -727,8 +763,14 @@
       <c r="Q7">
         <v>12237612.95833333</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="R7">
+        <v>5402</v>
+      </c>
+      <c r="S7">
+        <v>0.03082367591287649</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -780,8 +822,14 @@
       <c r="Q8">
         <v>12914346.16666667</v>
       </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="R8">
+        <v>6354</v>
+      </c>
+      <c r="S8">
+        <v>0.03088666625008012</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -833,8 +881,14 @@
       <c r="Q9">
         <v>11581358.45833333</v>
       </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="R9">
+        <v>5079</v>
+      </c>
+      <c r="S9">
+        <v>0.02841555478664241</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -886,8 +940,14 @@
       <c r="Q10">
         <v>12190737.58333333</v>
       </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="R10">
+        <v>5329</v>
+      </c>
+      <c r="S10">
+        <v>0.03237603515037423</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -939,8 +999,14 @@
       <c r="Q11">
         <v>12032276.79166667</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="R11">
+        <v>5218</v>
+      </c>
+      <c r="S11">
+        <v>0.02555287587939577</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -992,8 +1058,14 @@
       <c r="Q12">
         <v>11880239.75</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="R12">
+        <v>5383</v>
+      </c>
+      <c r="S12">
+        <v>0.03704010792859991</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1045,8 +1117,14 @@
       <c r="Q13">
         <v>12201524.58333333</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="R13">
+        <v>5654</v>
+      </c>
+      <c r="S13">
+        <v>0.03681209818587049</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1097,6 +1175,12 @@
       </c>
       <c r="Q14">
         <v>11779178.54166667</v>
+      </c>
+      <c r="R14">
+        <v>4574</v>
+      </c>
+      <c r="S14">
+        <v>0.02411168792458445</v>
       </c>
     </row>
   </sheetData>

</xml_diff>